<commit_message>
added generate report button.
</commit_message>
<xml_diff>
--- a/Backend/TestCompanyInputWorking7_2024_report_2024_8.xlsx
+++ b/Backend/TestCompanyInputWorking7_2024_report_2024_8.xlsx
@@ -482,7 +482,11 @@
           <t>Bob</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>01/01/2000</t>
+        </is>
+      </c>
       <c r="D2" t="inlineStr">
         <is>
           <t>C1</t>
@@ -516,7 +520,11 @@
           <t>Bob 2</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>01/01/1980</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>C1</t>
@@ -550,7 +558,11 @@
           <t>OtherGuy</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>01/01/1980</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
           <t>C1</t>

</xml_diff>